<commit_message>
Random Changes for FAR OUT
</commit_message>
<xml_diff>
--- a/MasterParameters.xlsx
+++ b/MasterParameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a0e4c4267ba78d20/Desktop/TheRocket/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryansmithers/Desktop/ProjectLiquid/TheRocket/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{812BFEFD-E54A-8348-9026-F6B9101C12CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A45A4A71-8192-421C-8F88-F2BAA7C1D921}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B09803-54D7-D14F-9D89-E56EB3584A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{C3C4CF6F-A6F1-7741-A638-B36B6E712D19}"/>
+    <workbookView xWindow="19660" yWindow="500" windowWidth="21180" windowHeight="23220" xr2:uid="{C3C4CF6F-A6F1-7741-A638-B36B6E712D19}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -759,18 +759,18 @@
   <dimension ref="B1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.5" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="14.296875" customWidth="1"/>
-    <col min="8" max="8" width="25.69921875" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>41</v>
       </c>
@@ -799,7 +799,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="49.05" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="2:10" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="32" t="s">
         <v>40</v>
       </c>
@@ -808,15 +808,15 @@
       <c r="E2" s="32"/>
       <c r="F2" s="32"/>
     </row>
-    <row r="3" spans="2:10" ht="16.05" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="32"/>
       <c r="C3" s="32"/>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
     </row>
-    <row r="4" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="38" t="s">
         <v>16</v>
       </c>
@@ -831,7 +831,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>29</v>
       </c>
@@ -854,12 +854,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="20" t="s">
         <v>37</v>
       </c>
       <c r="C7" s="21">
-        <v>5</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>33</v>
@@ -874,7 +874,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="23" t="s">
         <v>17</v>
       </c>
@@ -894,7 +894,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="23" t="s">
         <v>18</v>
       </c>
@@ -914,7 +914,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
       <c r="D10" s="3"/>
       <c r="F10" s="23" t="s">
@@ -927,7 +927,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
@@ -941,7 +941,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F12" s="23" t="s">
         <v>6</v>
       </c>
@@ -952,7 +952,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="41" t="s">
         <v>19</v>
       </c>
@@ -963,13 +963,13 @@
       </c>
       <c r="G13" s="34">
         <f>G15/G28</f>
-        <v>11.622418879056045</v>
+        <v>5.6972641564000233</v>
       </c>
       <c r="H13" s="29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
         <v>29</v>
       </c>
@@ -989,7 +989,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="20" t="s">
         <v>20</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="23" t="s">
         <v>21</v>
       </c>
@@ -1029,12 +1029,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="23" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="24">
-        <v>0.26369999999999999</v>
+        <v>0.29060000000000002</v>
       </c>
       <c r="D17" s="25" t="s">
         <v>32</v>
@@ -1049,12 +1049,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="24">
-        <v>0.1797</v>
+        <v>0.13719999999999999</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>32</v>
@@ -1069,7 +1069,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="23" t="s">
         <v>24</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="23" t="s">
         <v>25</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="D21" s="3"/>
       <c r="F21" s="23" t="s">
@@ -1122,7 +1122,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
       <c r="D22" s="6"/>
@@ -1130,8 +1130,8 @@
       <c r="G22" s="5"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="1"/>
       <c r="F24" s="44" t="s">
         <v>36</v>
@@ -1139,7 +1139,7 @@
       <c r="G24" s="45"/>
       <c r="H24" s="46"/>
     </row>
-    <row r="25" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F25" s="18" t="s">
         <v>29</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F26" s="20" t="s">
         <v>0</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F27" s="23" t="s">
         <v>1</v>
       </c>
@@ -1172,19 +1172,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F28" s="28" t="s">
         <v>35</v>
       </c>
       <c r="G28" s="30">
         <f>C7*G27/G26</f>
-        <v>2.1510152284263961</v>
+        <v>4.3880710659898474</v>
       </c>
       <c r="H28" s="31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F29" s="23" t="s">
         <v>15</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F30" s="23" t="s">
         <v>14</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F31" s="23" t="s">
         <v>13</v>
       </c>
@@ -1217,11 +1217,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="F32" s="2"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="6:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="6:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F33" s="4"/>
       <c r="G33" s="5"/>
       <c r="H33" s="6"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/Project-Liquid/TheRocket"
This reverts commit cdaa05bef08601f6ac46ec405f4c7452c3e1b349, reversing
changes made to 93c2fb4b9ba7a2fcd88f1c0881b652017d45a85b.
</commit_message>
<xml_diff>
--- a/MasterParameters.xlsx
+++ b/MasterParameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryansmithers/Desktop/ProjectLiquid/TheRocket/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaroncope/Desktop/TheRocket/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F6CCB5-A517-6D44-B9DB-73B82E3EAED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB079AB-83E0-904B-8FE8-8449ACAF38DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8140" yWindow="500" windowWidth="30860" windowHeight="24240" xr2:uid="{C3C4CF6F-A6F1-7741-A638-B36B6E712D19}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{C3C4CF6F-A6F1-7741-A638-B36B6E712D19}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -457,9 +457,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -497,7 +497,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -603,7 +603,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -745,7 +745,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -759,7 +759,7 @@
   <dimension ref="B1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -921,7 +921,7 @@
         <v>4</v>
       </c>
       <c r="G10" s="33">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H10" s="25" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Revert "Merge pull request #1 from Project-Liquid/main"
This reverts commit 6bef87dd192712809a8ffb9b667e4e8d3c5fbe26, reversing
changes made to 3a23b5860dc80085e7c564941fb7d16d8f26f3d8.
</commit_message>
<xml_diff>
--- a/MasterParameters.xlsx
+++ b/MasterParameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaroncope/Desktop/TheRocket/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryansmithers/Desktop/ProjectLiquid/TheRocket/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB079AB-83E0-904B-8FE8-8449ACAF38DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F6CCB5-A517-6D44-B9DB-73B82E3EAED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{C3C4CF6F-A6F1-7741-A638-B36B6E712D19}"/>
+    <workbookView xWindow="8140" yWindow="500" windowWidth="30860" windowHeight="24240" xr2:uid="{C3C4CF6F-A6F1-7741-A638-B36B6E712D19}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -457,9 +457,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -497,7 +497,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -603,7 +603,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -745,7 +745,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -759,7 +759,7 @@
   <dimension ref="B1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -921,7 +921,7 @@
         <v>4</v>
       </c>
       <c r="G10" s="33">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H10" s="25" t="s">
         <v>32</v>

</xml_diff>